<commit_message>
more horai gakuen items
</commit_message>
<xml_diff>
--- a/horai-school/checklist.xlsx
+++ b/horai-school/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/horai-school/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15721BC7-8DF1-E545-B2F9-3DF25F66085C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21912997-64A6-BD46-96F6-F0704BA87DD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{EBAC5F8B-C89D-914F-BBEA-4FE9DD3B39D8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{EBAC5F8B-C89D-914F-BBEA-4FE9DD3B39D8}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>year</t>
   </si>
@@ -117,6 +117,99 @@
   </si>
   <si>
     <t>rulebook</t>
+  </si>
+  <si>
+    <t>蓬莱学園DX1 改訂版リプレイ特集</t>
+  </si>
+  <si>
+    <t>Horai Gakuen DX1 Revised Replay Special</t>
+  </si>
+  <si>
+    <t>蓬莱学園DX2 特集・1995年学園祭</t>
+  </si>
+  <si>
+    <t>Horai Gakuen DX2 Special Feature / 1995 School Festival</t>
+  </si>
+  <si>
+    <t>SoftBank Creative</t>
+  </si>
+  <si>
+    <t>蓬莱学園DX3 蓬莱学園の授業・卒業</t>
+  </si>
+  <si>
+    <t>Horai Gakuen DX3 Horai Gakuen Class / Graduation</t>
+  </si>
+  <si>
+    <t>revised-replay.jpg</t>
+  </si>
+  <si>
+    <t>replay</t>
+  </si>
+  <si>
+    <t>revised-school-feature.jpg</t>
+  </si>
+  <si>
+    <t>revised-graduation.jpg</t>
+  </si>
+  <si>
+    <t>蓬莱学園ワールドツアー</t>
+  </si>
+  <si>
+    <t>Horai Gakuen World Tour</t>
+  </si>
+  <si>
+    <t>Shinkigensha</t>
+  </si>
+  <si>
+    <t>hourai_gakuen_world_tour.jpg</t>
+  </si>
+  <si>
+    <t>蓬莱生活事典　蓬莱学園の冒険！！ー改訂版ーサプリメント</t>
+  </si>
+  <si>
+    <t>Horai Life Encyclopedia: Adventure of Horai Gakuen! !! Revised version</t>
+  </si>
+  <si>
+    <t>horai_school_living_encyclopdedia.jpg</t>
+  </si>
+  <si>
+    <t>蓬莱学園人名事典</t>
+  </si>
+  <si>
+    <t>Horai Gakuen Biographical Dictionary</t>
+  </si>
+  <si>
+    <t>horai_gakuen_biographical_dictionary.jpg</t>
+  </si>
+  <si>
+    <t>なんでもかんでも蓬莱学園</t>
+  </si>
+  <si>
+    <t>BNN</t>
+  </si>
+  <si>
+    <t>Everything about Horai Gakuen</t>
+  </si>
+  <si>
+    <t>everything_about_horai_gakuen.jpg</t>
+  </si>
+  <si>
+    <t>試験に出る蓬莱学園!</t>
+  </si>
+  <si>
+    <t>Taking the Exam Horai Gakuen</t>
+  </si>
+  <si>
+    <t>taking_the_exam.jpg</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>Y-9101</t>
+  </si>
+  <si>
+    <t>Y-9104</t>
   </si>
 </sst>
 </file>
@@ -477,21 +570,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BBD45F-D764-D943-985E-9A9DA3A5777A}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" customWidth="1"/>
+    <col min="2" max="2" width="58.83203125" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +603,11 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1991</v>
       </c>
@@ -530,8 +626,11 @@
       <c r="F2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -548,7 +647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -565,7 +664,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1993</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -581,8 +683,11 @@
       <c r="F5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -599,7 +704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -617,6 +722,163 @@
       </c>
       <c r="F7" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1995</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1991</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1994</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1994</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1995</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1995</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1996</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweak english item name
</commit_message>
<xml_diff>
--- a/horai-school/checklist.xlsx
+++ b/horai-school/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/horai-school/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9160A909-6ACC-5341-8702-93EBC3EE9365}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD5FD4CE-F4A5-DC44-851E-2C5714E2B018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{EBAC5F8B-C89D-914F-BBEA-4FE9DD3B39D8}"/>
   </bookViews>
@@ -206,10 +206,10 @@
     <t>Y-9104</t>
   </si>
   <si>
-    <t>Horai Life Encyclopedia: Adventure of Horai Gakuen!! Revised version</t>
-  </si>
-  <si>
     <t>horai_school_living_encyclopedia.jpg</t>
+  </si>
+  <si>
+    <t>Horai Life Encyclopedia: Adventure of Horai Gakuen!! Revised Editio</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,13 +729,13 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>

</xml_diff>